<commit_message>
Login Seeding - revived
</commit_message>
<xml_diff>
--- a/Documents/users.xlsx
+++ b/Documents/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjo0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\kjo1\SN\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{225CE27C-B374-4962-B445-372E5A8D9860}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E46C8E7-AFCE-4DB1-BAB6-09A796CA7177}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40695" yWindow="2685" windowWidth="12150" windowHeight="15435" xr2:uid="{D43E3529-966F-4E15-B3A4-83DAAE253CF1}"/>
   </bookViews>
@@ -31,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>captain2@outlook.com</t>
-  </si>
-  <si>
-    <t>bnb</t>
   </si>
   <si>
     <t>captain</t>
@@ -417,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95ACBF4F-AE3F-43C1-B890-2A67D3336712}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,45 +425,33 @@
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>